<commit_message>
Adjust excel column widths for better printing
</commit_message>
<xml_diff>
--- a/src/template/Filterregnskap_template.xlsx
+++ b/src/template/Filterregnskap_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4A42E8-2C09-4721-9D82-C92C92C2CF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F8EF9E-F72A-4FC3-9E36-BF1E313E04E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -914,17 +914,15 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="55.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="2.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="60.44140625" style="2" customWidth="1"/>

</xml_diff>